<commit_message>
update in yml file
</commit_message>
<xml_diff>
--- a/output/bankrate.xlsx
+++ b/output/bankrate.xlsx
@@ -58,40 +58,40 @@
     <t>30-Year Fixed Rate Jumbo</t>
   </si>
   <si>
-    <t>6.58%</t>
-  </si>
-  <si>
-    <t>6.26%</t>
+    <t>6.67%</t>
+  </si>
+  <si>
+    <t>6.36%</t>
+  </si>
+  <si>
+    <t>5.85%</t>
   </si>
   <si>
     <t>5.76%</t>
   </si>
   <si>
-    <t>5.71%</t>
-  </si>
-  <si>
-    <t>6.31%</t>
-  </si>
-  <si>
-    <t>6.36%</t>
+    <t>6.56%</t>
   </si>
   <si>
     <t>6.66%</t>
   </si>
   <si>
-    <t>6.64%</t>
-  </si>
-  <si>
-    <t>6.35%</t>
-  </si>
-  <si>
-    <t>5.86%</t>
-  </si>
-  <si>
-    <t>5.79%</t>
-  </si>
-  <si>
-    <t>6.41%</t>
+    <t>6.73%</t>
+  </si>
+  <si>
+    <t>6.45%</t>
+  </si>
+  <si>
+    <t>5.94%</t>
+  </si>
+  <si>
+    <t>5.83%</t>
+  </si>
+  <si>
+    <t>6.61%</t>
+  </si>
+  <si>
+    <t>6.70%</t>
   </si>
   <si>
     <t>6.71%</t>
@@ -112,7 +112,7 @@
     <t>Bankrate</t>
   </si>
   <si>
-    <t>2025-08-08</t>
+    <t>2025-08-11</t>
   </si>
   <si>
     <t>Purchase</t>
@@ -510,7 +510,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
@@ -533,7 +533,7 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
@@ -556,7 +556,7 @@
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
@@ -579,7 +579,7 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
         <v>30</v>
@@ -602,7 +602,7 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
@@ -645,7 +645,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
small change in yml
</commit_message>
<xml_diff>
--- a/output/bankrate.xlsx
+++ b/output/bankrate.xlsx
@@ -58,48 +58,48 @@
     <t>30-Year Fixed Rate Jumbo</t>
   </si>
   <si>
-    <t>6.71%</t>
-  </si>
-  <si>
-    <t>6.39%</t>
-  </si>
-  <si>
-    <t>5.87%</t>
-  </si>
-  <si>
-    <t>5.78%</t>
-  </si>
-  <si>
-    <t>6.61%</t>
-  </si>
-  <si>
-    <t>6.78%</t>
-  </si>
-  <si>
-    <t>6.75%</t>
-  </si>
-  <si>
-    <t>6.77%</t>
-  </si>
-  <si>
-    <t>6.48%</t>
-  </si>
-  <si>
-    <t>5.96%</t>
+    <t>6.66%</t>
+  </si>
+  <si>
+    <t>6.33%</t>
   </si>
   <si>
     <t>5.86%</t>
   </si>
   <si>
-    <t>6.68%</t>
-  </si>
-  <si>
-    <t>6.82%</t>
+    <t>5.77%</t>
+  </si>
+  <si>
+    <t>6.73%</t>
+  </si>
+  <si>
+    <t>6.79%</t>
+  </si>
+  <si>
+    <t>6.65%</t>
+  </si>
+  <si>
+    <t>6.72%</t>
+  </si>
+  <si>
+    <t>6.42%</t>
+  </si>
+  <si>
+    <t>5.95%</t>
+  </si>
+  <si>
+    <t>5.85%</t>
   </si>
   <si>
     <t>6.80%</t>
   </si>
   <si>
+    <t>6.84%</t>
+  </si>
+  <si>
+    <t>6.69%</t>
+  </si>
+  <si>
     <t>30</t>
   </si>
   <si>
@@ -115,7 +115,7 @@
     <t>Bankrate</t>
   </si>
   <si>
-    <t>2025-08-12</t>
+    <t>2025-08-13</t>
   </si>
   <si>
     <t>Purchase</t>

</xml_diff>